<commit_message>
DEV-2004 Simplify Import Tasks - Remove Logstash
 - Update XLSX samples

Ticket:https://app.clickup.com/t/2304761/DEV-2004
</commit_message>
<xml_diff>
--- a/samples/bom_import_sample.xlsx
+++ b/samples/bom_import_sample.xlsx
@@ -52,10 +52,10 @@
     <t xml:space="preserve">component_qty</t>
   </si>
   <si>
-    <t xml:space="preserve">BOM 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test-sku-1</t>
+    <t xml:space="preserve">BOM 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-sku-6</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">test-sku-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test-sku-3</t>
+    <t xml:space="preserve">test-sku-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-sku-8</t>
   </si>
 </sst>
 </file>
@@ -82,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,17 +167,17 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.35"/>

</xml_diff>